<commit_message>
3/30/2023: Changed variance of the regression only model to 85.
</commit_message>
<xml_diff>
--- a/Results/Result Tables.xlsx
+++ b/Results/Result Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sjsu0-my.sharepoint.com/personal/peter_v_pham_sjsu_edu/Documents/Antithrombin Feature Extraction/Regression/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="237" documentId="8_{A47978B1-135A-4C6E-BA9C-AAFD41ED6B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F13119F-ABF1-405A-8C57-D3E7E856CF6A}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{A47978B1-135A-4C6E-BA9C-AAFD41ED6B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F90943D5-04A7-44FB-8BC0-CAF9FB64B158}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{80671288-5DE4-4F9B-BCCD-6896FA885FF8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{80671288-5DE4-4F9B-BCCD-6896FA885FF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,12 +173,6 @@
     <t>Regression only Models</t>
   </si>
   <si>
-    <t>Feature Count</t>
-  </si>
-  <si>
-    <t>Log Traiing RMSE</t>
-  </si>
-  <si>
     <t>Log Validation RMSE</t>
   </si>
   <si>
@@ -194,9 +188,6 @@
     <t>PCA w/90% Variance</t>
   </si>
   <si>
-    <t>PCA with 100% Variance</t>
-  </si>
-  <si>
     <t>PCA w/100% variance</t>
   </si>
   <si>
@@ -207,6 +198,15 @@
   </si>
   <si>
     <t>PCA w/85% Variance</t>
+  </si>
+  <si>
+    <t>Log Training RMSE</t>
+  </si>
+  <si>
+    <t>PCA w/95% Variance</t>
+  </si>
+  <si>
+    <t>Feature/PC Count</t>
   </si>
 </sst>
 </file>
@@ -454,10 +454,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A726633E-6673-4A2B-B032-A54798ADE8C8}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,7 +972,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H13" s="22" t="s">
         <v>15</v>
@@ -1088,7 +1088,7 @@
         <v>29</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>15</v>
@@ -1165,19 +1165,19 @@
         <v>35</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="O26" s="23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
@@ -1185,7 +1185,7 @@
         <v>33</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L27" s="1">
         <v>572</v>
@@ -1203,55 +1203,55 @@
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J28" s="8"/>
       <c r="K28" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L28" s="1">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="M28" s="1">
-        <v>1.0589999999999999</v>
+        <v>1.028</v>
       </c>
       <c r="N28" s="1">
-        <v>1.391</v>
+        <v>1.367</v>
       </c>
       <c r="O28" s="20">
-        <v>886836</v>
+        <v>1268435</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J29" s="8"/>
       <c r="K29" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L29" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M29" s="1">
-        <v>1.1779999999999999</v>
+        <v>1.0129999999999999</v>
       </c>
       <c r="N29" s="1">
-        <v>1.3360000000000001</v>
+        <v>1.2230000000000001</v>
       </c>
       <c r="O29" s="20">
-        <v>196397</v>
+        <v>474177</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J30" s="8"/>
       <c r="K30" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L30" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M30" s="1">
-        <v>1.089</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="N30" s="1">
-        <v>1.2969999999999999</v>
+        <v>1.2470000000000001</v>
       </c>
       <c r="O30" s="20">
-        <v>377884</v>
+        <v>269419</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
@@ -1259,7 +1259,7 @@
         <v>34</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L31" s="1">
         <v>572</v>
@@ -1277,16 +1277,16 @@
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J32" s="8"/>
       <c r="K32" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L32" s="1">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="M32" s="1">
-        <v>0.65100000000000002</v>
+        <v>0.625</v>
       </c>
       <c r="N32" s="1">
-        <v>1.411</v>
+        <v>1.379</v>
       </c>
       <c r="O32" s="20">
         <v>503180</v>
@@ -1295,19 +1295,19 @@
     <row r="33" spans="10:15" x14ac:dyDescent="0.35">
       <c r="J33" s="8"/>
       <c r="K33" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L33" s="1">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="M33" s="1">
-        <v>0.65100000000000002</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="N33" s="1">
-        <v>1.411</v>
+        <v>1.379</v>
       </c>
       <c r="O33" s="20">
-        <v>503495</v>
+        <v>181460</v>
       </c>
     </row>
     <row r="34" spans="10:15" x14ac:dyDescent="0.35">
@@ -1315,7 +1315,7 @@
         <v>32</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L34" s="1">
         <v>572</v>
@@ -1333,7 +1333,7 @@
     <row r="35" spans="10:15" x14ac:dyDescent="0.35">
       <c r="J35" s="8"/>
       <c r="K35" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L35" s="1">
         <v>28</v>
@@ -1351,7 +1351,7 @@
     <row r="36" spans="10:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J36" s="9"/>
       <c r="K36" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L36" s="5">
         <v>27</v>

</xml_diff>